<commit_message>
Eliminada columna T.SEG y renombrada a TSEGUI
</commit_message>
<xml_diff>
--- a/src/frontend/resources/plantilla_datos_pacientes.xlsx
+++ b/src/frontend/resources/plantilla_datos_pacientes.xlsx
@@ -5,22 +5,22 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hlocal\TFG\src\frontend\patients\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hlocal\TFG\src\frontend\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44BBFBB-DF4F-40DF-A1D1-43FEF81D43F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C708FD-F327-4C6B-8FB9-E56070049384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="100" windowWidth="14830" windowHeight="10240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="plantilla_datos_pacientes" sheetId="1" r:id="rId1"/>
+    <sheet name="Pacientes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>N</t>
   </si>
@@ -157,16 +157,13 @@
     <t>FECHAFIN</t>
   </si>
   <si>
-    <t>T.SEG</t>
+    <t>TSEGUI</t>
   </si>
   <si>
     <t>FALLEC</t>
   </si>
   <si>
     <t>TSUPERV</t>
-  </si>
-  <si>
-    <t>TSEGUI</t>
   </si>
   <si>
     <t>PSAFIN</t>
@@ -554,13 +551,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BM1"/>
+  <dimension ref="A1:BL1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AW6" sqref="AW6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -752,9 +751,6 @@
       </c>
       <c r="BL1" t="s">
         <v>63</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>